<commit_message>
Modificado menu en archivo excel
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="PhotoSOC" sheetId="2" r:id="rId1"/>
+    <sheet name="PhotoSOC" sheetId="3" r:id="rId1"/>
     <sheet name="Photoduino V0.9" sheetId="1" r:id="rId2"/>
+    <sheet name="PhotoSOC Old" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="79">
   <si>
     <t>&gt;Menú principal</t>
   </si>
@@ -240,6 +241,18 @@
   </si>
   <si>
     <t>3.Conf. Flashes</t>
+  </si>
+  <si>
+    <t>On/Off</t>
+  </si>
+  <si>
+    <t>Disp.Unico</t>
+  </si>
+  <si>
+    <t>T entre Disparos</t>
+  </si>
+  <si>
+    <t>Num.Disparos</t>
   </si>
 </sst>
 </file>
@@ -571,249 +584,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H41"/>
+  <dimension ref="B2:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:6">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:6">
       <c r="C3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:6">
       <c r="D4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:6">
       <c r="D5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:6">
       <c r="D6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:6">
       <c r="D7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="C9" t="s">
+    <row r="8" spans="2:6">
+      <c r="C8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
-      <c r="D10" t="s">
+    <row r="9" spans="2:6">
+      <c r="D9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="10" spans="2:6">
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
       <c r="E11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="E12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="E13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="12" spans="2:6">
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
       <c r="E14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:6">
       <c r="F15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
       <c r="F16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8">
-      <c r="F17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="3:8">
-      <c r="E18" t="s">
+    <row r="17" spans="3:6">
+      <c r="E17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="3:8">
-      <c r="D19" t="s">
+    <row r="18" spans="3:6">
+      <c r="D18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="3:8">
+    <row r="19" spans="3:6">
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
       <c r="E20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8">
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8">
-      <c r="E22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="3:8">
+    <row r="21" spans="3:6">
+      <c r="F21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
       <c r="E23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="3:8">
+    <row r="24" spans="3:6">
       <c r="F24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6">
       <c r="F25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8">
-      <c r="F26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="3:8">
-      <c r="E27" t="s">
+    <row r="26" spans="3:6">
+      <c r="E26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="3:8">
-      <c r="C28" t="s">
+    <row r="27" spans="3:6">
+      <c r="C27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="3:8">
+    <row r="28" spans="3:6">
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6">
       <c r="D29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6">
       <c r="D30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6">
       <c r="D31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8">
-      <c r="D32" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="3:7">
-      <c r="C33" t="s">
+      <c r="E31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="3:7">
-      <c r="D34" t="s">
+    <row r="33" spans="3:6">
+      <c r="D33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="3:7">
+    <row r="34" spans="3:6">
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6">
       <c r="D35" t="s">
-        <v>57</v>
-      </c>
-      <c r="G35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7">
-      <c r="C36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6">
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6">
       <c r="D37" t="s">
-        <v>2</v>
-      </c>
-      <c r="G37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7">
-      <c r="D38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7">
-      <c r="D39" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7">
-      <c r="D40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7">
-      <c r="D41" t="s">
         <v>58</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F37" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1367,4 +1347,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:H41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="44.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8">
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8">
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8">
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8">
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8">
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8">
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8">
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8">
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8">
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8">
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8">
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7">
+      <c r="D38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>